<commit_message>
update experimental results for multiple coverages with different slicing
</commit_message>
<xml_diff>
--- a/experiment_results/coverage_100___AGGREGATION_ARITHMETIC_MEAN_NORMALIZATION_ALPHA_BETA/ExamDB/4wise/0.0_.xlsx
+++ b/experiment_results/coverage_100___AGGREGATION_ARITHMETIC_MEAN_NORMALIZATION_ALPHA_BETA/ExamDB/4wise/0.0_.xlsx
@@ -632,13 +632,13 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -673,13 +673,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>19</v>
@@ -714,13 +714,13 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -755,13 +755,13 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -796,13 +796,13 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>14</v>
@@ -837,13 +837,13 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -878,13 +878,13 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>16</v>
@@ -919,13 +919,13 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>16</v>
@@ -960,13 +960,13 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>11</v>
@@ -1001,13 +1001,13 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -1042,13 +1042,13 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -1083,13 +1083,13 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -1124,13 +1124,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -1165,13 +1165,13 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -1206,13 +1206,13 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -1247,13 +1247,13 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
       <c r="E17">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1288,13 +1288,13 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1329,13 +1329,13 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -1370,13 +1370,13 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -1411,13 +1411,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>11</v>
@@ -1452,13 +1452,13 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -1493,13 +1493,13 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>4</v>
@@ -1534,13 +1534,13 @@
         <v>56</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1575,13 +1575,13 @@
         <v>58</v>
       </c>
       <c r="C25">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D25">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>16</v>
@@ -1616,13 +1616,13 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -1657,13 +1657,13 @@
         <v>62</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>16</v>
@@ -1698,13 +1698,13 @@
         <v>64</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>11</v>
@@ -1739,13 +1739,13 @@
         <v>66</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>12</v>
@@ -1780,13 +1780,13 @@
         <v>68</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E30">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>5</v>
@@ -1821,13 +1821,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>8</v>
@@ -1862,13 +1862,13 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="D32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E32">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -1903,13 +1903,13 @@
         <v>74</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -1944,13 +1944,13 @@
         <v>76</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>14</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>14</v>
@@ -2036,13 +2036,13 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -2077,13 +2077,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -2118,13 +2118,13 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -2159,13 +2159,13 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -2200,13 +2200,13 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -2241,13 +2241,13 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -2282,13 +2282,13 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -2323,13 +2323,13 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -2364,13 +2364,13 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -2405,13 +2405,13 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -2446,13 +2446,13 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -2487,13 +2487,13 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -2528,13 +2528,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -2569,13 +2569,13 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -2610,13 +2610,13 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -2651,13 +2651,13 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -2692,13 +2692,13 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -2733,13 +2733,13 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -2774,13 +2774,13 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -2815,13 +2815,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -2856,13 +2856,13 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>14</v>
@@ -2897,13 +2897,13 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -2938,13 +2938,13 @@
         <v>56</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -2979,13 +2979,13 @@
         <v>58</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -3020,13 +3020,13 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3061,13 +3061,13 @@
         <v>62</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -3102,13 +3102,13 @@
         <v>64</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>9</v>
@@ -3143,13 +3143,13 @@
         <v>66</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -3184,13 +3184,13 @@
         <v>68</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -3225,13 +3225,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -3266,13 +3266,13 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -3307,13 +3307,13 @@
         <v>74</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -3348,13 +3348,13 @@
         <v>76</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>3</v>
@@ -3440,13 +3440,13 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -3481,13 +3481,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3522,13 +3522,13 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3563,13 +3563,13 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3604,13 +3604,13 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -3645,13 +3645,13 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -3686,13 +3686,13 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -3727,13 +3727,13 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -3768,13 +3768,13 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -3809,13 +3809,13 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -3850,13 +3850,13 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -3891,13 +3891,13 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -3932,13 +3932,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -3973,13 +3973,13 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -4014,13 +4014,13 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -4055,13 +4055,13 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -4096,13 +4096,13 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -4137,13 +4137,13 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -4178,13 +4178,13 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -4219,13 +4219,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -4260,13 +4260,13 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>-1</v>
       </c>
       <c r="D22">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>28</v>
@@ -4301,13 +4301,13 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -4342,13 +4342,13 @@
         <v>56</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -4383,13 +4383,13 @@
         <v>58</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -4424,13 +4424,13 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -4465,13 +4465,13 @@
         <v>62</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -4506,13 +4506,13 @@
         <v>64</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>9</v>
@@ -4547,13 +4547,13 @@
         <v>66</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -4588,13 +4588,13 @@
         <v>68</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -4629,13 +4629,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -4670,13 +4670,13 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -4711,13 +4711,13 @@
         <v>74</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -4752,13 +4752,13 @@
         <v>76</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>3</v>
@@ -4844,13 +4844,13 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -4885,13 +4885,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>19</v>
@@ -4926,13 +4926,13 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -4967,13 +4967,13 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -5008,13 +5008,13 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>14</v>
@@ -5049,13 +5049,13 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -5090,13 +5090,13 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>16</v>
@@ -5131,13 +5131,13 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>16</v>
@@ -5172,13 +5172,13 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>11</v>
@@ -5213,13 +5213,13 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -5254,13 +5254,13 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -5295,13 +5295,13 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -5336,13 +5336,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -5377,13 +5377,13 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -5418,13 +5418,13 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -5459,13 +5459,13 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
       <c r="E17">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -5500,13 +5500,13 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -5541,13 +5541,13 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -5582,13 +5582,13 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -5623,13 +5623,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>11</v>
@@ -5664,13 +5664,13 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -5705,13 +5705,13 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>4</v>
@@ -5746,13 +5746,13 @@
         <v>56</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -5787,13 +5787,13 @@
         <v>58</v>
       </c>
       <c r="C25">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D25">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>16</v>
@@ -5828,13 +5828,13 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -5869,13 +5869,13 @@
         <v>62</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>16</v>
@@ -5910,13 +5910,13 @@
         <v>64</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>11</v>
@@ -5951,13 +5951,13 @@
         <v>66</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>12</v>
@@ -5992,13 +5992,13 @@
         <v>68</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E30">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>5</v>
@@ -6033,13 +6033,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>8</v>
@@ -6074,13 +6074,13 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="D32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E32">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -6115,13 +6115,13 @@
         <v>74</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -6156,13 +6156,13 @@
         <v>76</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>14</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>14</v>
@@ -6248,13 +6248,13 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -6289,13 +6289,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -6330,13 +6330,13 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -6371,13 +6371,13 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -6412,13 +6412,13 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -6453,13 +6453,13 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -6494,13 +6494,13 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -6535,13 +6535,13 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -6576,13 +6576,13 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -6617,13 +6617,13 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -6658,13 +6658,13 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -6699,13 +6699,13 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -6740,13 +6740,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -6781,13 +6781,13 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -6822,13 +6822,13 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -6863,13 +6863,13 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -6904,13 +6904,13 @@
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -6945,13 +6945,13 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -6986,13 +6986,13 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -7027,13 +7027,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -7068,13 +7068,13 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="D22">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>20</v>
@@ -7109,13 +7109,13 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -7150,13 +7150,13 @@
         <v>56</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -7191,13 +7191,13 @@
         <v>58</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -7232,13 +7232,13 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -7273,13 +7273,13 @@
         <v>62</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -7314,13 +7314,13 @@
         <v>64</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>9</v>
@@ -7355,13 +7355,13 @@
         <v>66</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -7396,13 +7396,13 @@
         <v>68</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -7437,13 +7437,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -7478,13 +7478,13 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -7519,13 +7519,13 @@
         <v>74</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -7560,13 +7560,13 @@
         <v>76</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>3</v>

</xml_diff>